<commit_message>
Search + Desain Endpoint
</commit_message>
<xml_diff>
--- a/Checklist Endpoint.xlsx
+++ b/Checklist Endpoint.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincent\Documents\KULIAH\SOA\proyek-soa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Tjen\Documents\BACKUP\KULIAH\SEMESTER 6\SOA\Proyek SOA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D4FFBA-6DEE-42EA-9AE6-4D6C1785C1EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7FC01D8-EF2B-4911-BC23-71C939A1F2C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="63">
   <si>
     <t>METHOD</t>
   </si>
@@ -75,36 +75,18 @@
     <t>GET</t>
   </si>
   <si>
-    <t>/search/:keyword</t>
-  </si>
-  <si>
     <t>/user/:username</t>
   </si>
   <si>
     <t>Mencari bookshelf sesuai dengan username</t>
   </si>
   <si>
-    <t>/playlist/user/:username</t>
-  </si>
-  <si>
-    <t>/playlist/name/:name</t>
-  </si>
-  <si>
-    <t>Mencari playlist berdasarkan nama playlist</t>
-  </si>
-  <si>
     <t>/user/:keyword</t>
   </si>
   <si>
     <t>Mencari user berdasarkan keyword dari username</t>
   </si>
   <si>
-    <t>Mencari buku berdasarkan keyword dari judul buku</t>
-  </si>
-  <si>
-    <t>Mencari playlist berdasarkan username dari pembuat playlist</t>
-  </si>
-  <si>
     <t>/bookmark/:id_buku</t>
   </si>
   <si>
@@ -165,9 +147,6 @@
     <t>/search/id/:id_buku</t>
   </si>
   <si>
-    <t>/user/:id_buku</t>
-  </si>
-  <si>
     <t>/user/upgrade</t>
   </si>
   <si>
@@ -192,9 +171,6 @@
     <t>v</t>
   </si>
   <si>
-    <t>/review/:query</t>
-  </si>
-  <si>
     <t>Menampilkan review sesuai dengan query</t>
   </si>
   <si>
@@ -214,13 +190,37 @@
   </si>
   <si>
     <t>Delete user</t>
+  </si>
+  <si>
+    <t>Menampilkan playlist sesuai dengan query</t>
+  </si>
+  <si>
+    <t>/playlist/detail/:id_playlist</t>
+  </si>
+  <si>
+    <t>Menampilkan list buku dari playlist berdasarkan id playlist</t>
+  </si>
+  <si>
+    <t>/playlist/self</t>
+  </si>
+  <si>
+    <t>/playlist/?query</t>
+  </si>
+  <si>
+    <t>/review/?query</t>
+  </si>
+  <si>
+    <t>/search/?query&amp;page</t>
+  </si>
+  <si>
+    <t>Mencari buku berdasarkan query dari judul dan penulis buku</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,13 +228,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -246,16 +258,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -568,21 +583,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" customWidth="1"/>
+    <col min="2" max="2" width="30.109375" customWidth="1"/>
+    <col min="3" max="3" width="27.44140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -593,10 +608,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -606,11 +621,11 @@
       <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D2" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -620,25 +635,25 @@
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D4" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -648,11 +663,11 @@
       <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D5" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -663,7 +678,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -674,324 +689,319 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="D12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>15</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D13" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D22" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26" t="s">
-        <v>47</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D26" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>36</v>
-      </c>
-      <c r="B27" t="s">
-        <v>61</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D27" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>36</v>
-      </c>
-      <c r="B28" t="s">
-        <v>30</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D28" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29" t="s">
-        <v>40</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>36</v>
-      </c>
-      <c r="B30" t="s">
-        <v>32</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>36</v>
-      </c>
-      <c r="B31" t="s">
-        <v>26</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D31" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>36</v>
-      </c>
-      <c r="B32" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D32" t="s">
-        <v>54</v>
+      <c r="D31" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>